<commit_message>
[ASSIGN7] Updated readme for ex01
</commit_message>
<xml_diff>
--- a/assignment_07/output/measurments.xlsx
+++ b/assignment_07/output/measurments.xlsx
@@ -8,46 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidedesclavis/Documents/WS-2020:21/ParalleleSysteme/GIT/parallel_systems/assignment_07/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB8D6F57-E821-B54B-B244-24875202D83B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED36944D-4A88-A24E-AEC0-4FEADB1BC438}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="28040" windowHeight="16620" xr2:uid="{0F7DCCF8-7CF4-1747-BDD2-80E395E22F32}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28040" windowHeight="16620" xr2:uid="{0F7DCCF8-7CF4-1747-BDD2-80E395E22F32}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Tabelle1!$A$120:$A$135</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Tabelle1!$B$119</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Tabelle1!$A$120:$A$135</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Tabelle1!$B$119</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Tabelle1!$B$120:$B$135</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Tabelle1!$C$119</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Tabelle1!$C$120:$C$135</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Tabelle1!$B$120:$B$135</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">Tabelle1!$A$120:$A$135</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">Tabelle1!$B$119</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">Tabelle1!$B$120:$B$135</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">Tabelle1!$C$119</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">Tabelle1!$C$120:$C$135</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Tabelle1!$C$119</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Tabelle1!$C$120:$C$135</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Tabelle1!$A$120:$A$135</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Tabelle1!$B$119</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Tabelle1!$B$120:$B$135</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Tabelle1!$C$119</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Tabelle1!$C$120:$C$135</definedName>
-    <definedName name="_xlchart.v2.15" hidden="1">Tabelle1!$A$120:$A$135</definedName>
-    <definedName name="_xlchart.v2.16" hidden="1">Tabelle1!$B$119</definedName>
-    <definedName name="_xlchart.v2.17" hidden="1">Tabelle1!$B$120:$B$135</definedName>
-    <definedName name="_xlchart.v2.18" hidden="1">Tabelle1!$C$119</definedName>
-    <definedName name="_xlchart.v2.19" hidden="1">Tabelle1!$C$120:$C$135</definedName>
-    <definedName name="_xlchart.v2.20" hidden="1">Tabelle1!$A$120:$A$135</definedName>
-    <definedName name="_xlchart.v2.21" hidden="1">Tabelle1!$B$119</definedName>
-    <definedName name="_xlchart.v2.22" hidden="1">Tabelle1!$B$120:$B$135</definedName>
-    <definedName name="_xlchart.v2.23" hidden="1">Tabelle1!$C$119</definedName>
-    <definedName name="_xlchart.v2.24" hidden="1">Tabelle1!$C$120:$C$135</definedName>
-  </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -235,10 +203,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="166" formatCode="#,##0.0000"/>
-    <numFmt numFmtId="167" formatCode="#,##0.00000"/>
-    <numFmt numFmtId="168" formatCode="#,##0.000000"/>
-    <numFmt numFmtId="178" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00000"/>
+    <numFmt numFmtId="166" formatCode="#,##0.000000"/>
+    <numFmt numFmtId="167" formatCode="0.000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -371,28 +339,33 @@
   </cellStyleXfs>
   <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -402,11 +375,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1111,16 +1079,13 @@
               <a:buFontTx/>
               <a:buNone/>
               <a:tabLst/>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr>
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:sysClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="de-DE"/>
@@ -7193,8 +7158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C37CDA07-DB48-0449-A657-8D4C3881F8A1}">
   <dimension ref="A2:W191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A132" workbookViewId="0">
-      <selection activeCell="O149" sqref="O149"/>
+    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="A119" sqref="A119:C135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7281,87 +7246,87 @@
         <v>9</v>
       </c>
       <c r="B4" s="10">
-        <f>(B185+B190)/2</f>
+        <f t="shared" ref="B4:V4" si="0">(B185+B190)/2</f>
         <v>4.0653349999999993</v>
       </c>
       <c r="C4" s="7">
-        <f>(C185+C190)/2</f>
+        <f t="shared" si="0"/>
         <v>4.1290750000000003</v>
       </c>
       <c r="D4" s="8">
-        <f>(D185+D190)/2</f>
+        <f t="shared" si="0"/>
         <v>2.13856</v>
       </c>
       <c r="E4" s="8">
-        <f>(E185+E190)/2</f>
+        <f t="shared" si="0"/>
         <v>3.1379899999999998</v>
       </c>
       <c r="F4" s="8">
-        <f>(F185+F190)/2</f>
+        <f t="shared" si="0"/>
         <v>2.8668449999999996</v>
       </c>
       <c r="G4" s="10">
-        <f>(G185+G190)/2</f>
+        <f t="shared" si="0"/>
         <v>1.0667550000000001</v>
       </c>
       <c r="H4" s="10">
-        <f>(H185+H190)/2</f>
+        <f t="shared" si="0"/>
         <v>2.5254950000000003</v>
       </c>
       <c r="I4" s="10">
-        <f>(I185+I190)/2</f>
+        <f t="shared" si="0"/>
         <v>2.2347350000000001</v>
       </c>
       <c r="J4" s="10">
-        <f>(J185+J190)/2</f>
+        <f t="shared" si="0"/>
         <v>0.76718249999999999</v>
       </c>
       <c r="K4" s="10">
-        <f>(K185+K190)/2</f>
+        <f t="shared" si="0"/>
         <v>2.1105999999999998</v>
       </c>
       <c r="L4" s="10">
-        <f>(L185+L190)/2</f>
+        <f t="shared" si="0"/>
         <v>1.806945</v>
       </c>
       <c r="M4" s="10">
-        <f>(M185+M190)/2</f>
+        <f t="shared" si="0"/>
         <v>0.60458849999999997</v>
       </c>
       <c r="N4" s="10">
-        <f>(N185+N190)/2</f>
+        <f t="shared" si="0"/>
         <v>1.4680900000000001</v>
       </c>
       <c r="O4" s="10">
-        <f>(O185+O190)/2</f>
+        <f t="shared" si="0"/>
         <v>1.5997950000000001</v>
       </c>
       <c r="P4" s="10">
-        <f>(P185+P190)/2</f>
+        <f t="shared" si="0"/>
         <v>0.47675699999999999</v>
       </c>
       <c r="Q4" s="10">
-        <f>(Q185+Q190)/2</f>
+        <f t="shared" si="0"/>
         <v>1.2944599999999999</v>
       </c>
       <c r="R4" s="10">
-        <f>(R185+R190)/2</f>
+        <f t="shared" si="0"/>
         <v>1.4374500000000001</v>
       </c>
       <c r="S4" s="10">
-        <f>(S185+S190)/2</f>
+        <f t="shared" si="0"/>
         <v>0.47568149999999998</v>
       </c>
       <c r="T4" s="10">
-        <f>(T185+T190)/2</f>
+        <f t="shared" si="0"/>
         <v>1.35487</v>
       </c>
       <c r="U4" s="10">
-        <f>(U185+U190)/2</f>
+        <f t="shared" si="0"/>
         <v>1.350635</v>
       </c>
       <c r="V4" s="10">
-        <f>(V185+V190)/2</f>
+        <f t="shared" si="0"/>
         <v>0.73123499999999997</v>
       </c>
       <c r="W4" s="15">
@@ -7374,87 +7339,87 @@
         <v>10</v>
       </c>
       <c r="B5" s="10">
-        <f>(B186+B191)/2</f>
+        <f t="shared" ref="B5:V5" si="1">(B186+B191)/2</f>
         <v>3.9895899999999997</v>
       </c>
       <c r="C5" s="7">
-        <f>(C186+C191)/2</f>
+        <f t="shared" si="1"/>
         <v>4.0861800000000006</v>
       </c>
       <c r="D5" s="8">
-        <f>(D186+D191)/2</f>
+        <f t="shared" si="1"/>
         <v>2.1298849999999998</v>
       </c>
       <c r="E5" s="8">
-        <f>(E186+E191)/2</f>
+        <f t="shared" si="1"/>
         <v>2.6284549999999998</v>
       </c>
       <c r="F5" s="8">
-        <f>(F186+F191)/2</f>
+        <f t="shared" si="1"/>
         <v>2.8059149999999997</v>
       </c>
       <c r="G5" s="10">
-        <f>(G186+G191)/2</f>
+        <f t="shared" si="1"/>
         <v>2.7487199999999996</v>
       </c>
       <c r="H5" s="10">
-        <f>(H186+H191)/2</f>
+        <f t="shared" si="1"/>
         <v>2.0141200000000001</v>
       </c>
       <c r="I5" s="10">
-        <f>(I186+I191)/2</f>
+        <f t="shared" si="1"/>
         <v>2.1045400000000001</v>
       </c>
       <c r="J5" s="10">
-        <f>(J186+J191)/2</f>
+        <f t="shared" si="1"/>
         <v>2.9574499999999997</v>
       </c>
       <c r="K5" s="10">
-        <f>(K186+K191)/2</f>
+        <f t="shared" si="1"/>
         <v>1.6816949999999999</v>
       </c>
       <c r="L5" s="10">
-        <f>(L186+L191)/2</f>
+        <f t="shared" si="1"/>
         <v>1.7452449999999999</v>
       </c>
       <c r="M5" s="10">
-        <f>(M186+M191)/2</f>
+        <f t="shared" si="1"/>
         <v>5.4897499999999999</v>
       </c>
       <c r="N5" s="10">
-        <f>(N186+N191)/2</f>
+        <f t="shared" si="1"/>
         <v>1.403335</v>
       </c>
       <c r="O5" s="10">
-        <f>(O186+O191)/2</f>
+        <f t="shared" si="1"/>
         <v>1.47055</v>
       </c>
       <c r="P5" s="10">
-        <f>(P186+P191)/2</f>
+        <f t="shared" si="1"/>
         <v>8.1544150000000002</v>
       </c>
       <c r="Q5" s="10">
-        <f>(Q186+Q191)/2</f>
+        <f t="shared" si="1"/>
         <v>1.2287300000000001</v>
       </c>
       <c r="R5" s="10">
-        <f>(R186+R191)/2</f>
+        <f t="shared" si="1"/>
         <v>1.3076300000000001</v>
       </c>
       <c r="S5" s="10">
-        <f>(S186+S191)/2</f>
+        <f t="shared" si="1"/>
         <v>11.4543</v>
       </c>
       <c r="T5" s="10">
-        <f>(T186+T191)/2</f>
+        <f t="shared" si="1"/>
         <v>1.0978349999999999</v>
       </c>
       <c r="U5" s="10">
-        <f>(U186+U191)/2</f>
+        <f t="shared" si="1"/>
         <v>1.1838099999999998</v>
       </c>
       <c r="V5" s="10">
-        <f>(V186+V191)/2</f>
+        <f t="shared" si="1"/>
         <v>15.652950000000001</v>
       </c>
       <c r="W5" s="15">
@@ -7463,31 +7428,31 @@
       </c>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A44" s="23" t="s">
+      <c r="A44" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="B44" s="23"/>
-      <c r="C44" s="23"/>
-      <c r="D44" s="23"/>
-      <c r="E44" s="23"/>
-      <c r="F44" s="23"/>
-      <c r="G44" s="23"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
-      <c r="K44" s="23"/>
-      <c r="L44" s="23"/>
-      <c r="M44" s="23"/>
-      <c r="N44" s="23"/>
-      <c r="O44" s="23"/>
-      <c r="P44" s="23"/>
-      <c r="Q44" s="23"/>
-      <c r="R44" s="23"/>
-      <c r="S44" s="23"/>
-      <c r="T44" s="23"/>
-      <c r="U44" s="23"/>
-      <c r="V44" s="23"/>
-      <c r="W44" s="23"/>
+      <c r="B44" s="28"/>
+      <c r="C44" s="28"/>
+      <c r="D44" s="28"/>
+      <c r="E44" s="28"/>
+      <c r="F44" s="28"/>
+      <c r="G44" s="28"/>
+      <c r="H44" s="28"/>
+      <c r="I44" s="28"/>
+      <c r="J44" s="28"/>
+      <c r="K44" s="28"/>
+      <c r="L44" s="28"/>
+      <c r="M44" s="28"/>
+      <c r="N44" s="28"/>
+      <c r="O44" s="28"/>
+      <c r="P44" s="28"/>
+      <c r="Q44" s="28"/>
+      <c r="R44" s="28"/>
+      <c r="S44" s="28"/>
+      <c r="T44" s="28"/>
+      <c r="U44" s="28"/>
+      <c r="V44" s="28"/>
+      <c r="W44" s="28"/>
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A45" s="21"/>
@@ -7727,26 +7692,26 @@
       <c r="W48" s="3"/>
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A84" s="23" t="s">
+      <c r="A84" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="B84" s="23"/>
-      <c r="C84" s="23"/>
-      <c r="D84" s="23"/>
-      <c r="E84" s="23"/>
-      <c r="F84" s="23"/>
-      <c r="G84" s="23"/>
-      <c r="H84" s="23"/>
-      <c r="I84" s="23"/>
-      <c r="J84" s="24" t="s">
+      <c r="B84" s="28"/>
+      <c r="C84" s="28"/>
+      <c r="D84" s="28"/>
+      <c r="E84" s="28"/>
+      <c r="F84" s="28"/>
+      <c r="G84" s="28"/>
+      <c r="H84" s="28"/>
+      <c r="I84" s="28"/>
+      <c r="J84" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="K84" s="25"/>
-      <c r="L84" s="25"/>
-      <c r="M84" s="25"/>
-      <c r="N84" s="25"/>
-      <c r="O84" s="25"/>
-      <c r="P84" s="25"/>
+      <c r="K84" s="30"/>
+      <c r="L84" s="30"/>
+      <c r="M84" s="30"/>
+      <c r="N84" s="30"/>
+      <c r="O84" s="30"/>
+      <c r="P84" s="30"/>
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A85" s="13"/>
@@ -7921,187 +7886,187 @@
       <c r="V118" s="18"/>
     </row>
     <row r="119" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A119" s="26"/>
-      <c r="B119" s="26" t="s">
+      <c r="A119" s="23"/>
+      <c r="B119" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="C119" s="26" t="s">
+      <c r="C119" s="23" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="120" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A120" s="27" t="s">
+      <c r="A120" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="B120" s="26">
+      <c r="B120" s="23">
         <v>5.7813299999999996</v>
       </c>
-      <c r="C120" s="26">
+      <c r="C120" s="23">
         <v>5.7101800000000003</v>
       </c>
     </row>
     <row r="121" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A121" s="28" t="s">
+      <c r="A121" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="B121" s="30">
+      <c r="B121" s="27">
         <v>3.9950600000000001</v>
       </c>
-      <c r="C121" s="26">
+      <c r="C121" s="23">
         <v>3.9948100000000002</v>
       </c>
     </row>
     <row r="122" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A122" s="28" t="s">
+      <c r="A122" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="B122" s="29">
+      <c r="B122" s="26">
         <v>2.7426300000000001</v>
       </c>
-      <c r="C122" s="29">
+      <c r="C122" s="26">
         <v>2.7383099999999998</v>
       </c>
     </row>
     <row r="123" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A123" s="28" t="s">
+      <c r="A123" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="B123" s="29">
+      <c r="B123" s="26">
         <v>2.1866400000000001</v>
       </c>
-      <c r="C123" s="29">
+      <c r="C123" s="26">
         <v>2.1952799999999999</v>
       </c>
     </row>
     <row r="124" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A124" s="27" t="s">
+      <c r="A124" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="B124" s="26">
+      <c r="B124" s="23">
         <v>3.0172300000000001</v>
       </c>
-      <c r="C124" s="26">
+      <c r="C124" s="23">
         <v>2.9867400000000002</v>
       </c>
     </row>
     <row r="125" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A125" s="28" t="s">
+      <c r="A125" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="B125" s="29">
+      <c r="B125" s="26">
         <v>4.0346900000000003</v>
       </c>
-      <c r="C125" s="29">
+      <c r="C125" s="26">
         <v>4.1189799999999996</v>
       </c>
     </row>
     <row r="126" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A126" s="28" t="s">
+      <c r="A126" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="B126" s="29">
+      <c r="B126" s="26">
         <v>2.1243599999999998</v>
       </c>
-      <c r="C126" s="29">
+      <c r="C126" s="26">
         <v>2.1967099999999999</v>
       </c>
     </row>
     <row r="127" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A127" s="27" t="s">
+      <c r="A127" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="B127" s="26">
+      <c r="B127" s="23">
         <v>2.0819800000000002</v>
       </c>
-      <c r="C127" s="26">
+      <c r="C127" s="23">
         <v>2.0572699999999999</v>
       </c>
     </row>
     <row r="128" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A128" s="28" t="s">
+      <c r="A128" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="B128" s="29">
+      <c r="B128" s="26">
         <v>2.7738100000000001</v>
       </c>
-      <c r="C128" s="29">
+      <c r="C128" s="26">
         <v>2.8153600000000001</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A129" s="28" t="s">
+      <c r="A129" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="B129" s="26">
+      <c r="B129" s="23">
         <v>1.4618500000000001</v>
       </c>
-      <c r="C129" s="26">
+      <c r="C129" s="23">
         <v>4.2286200000000003</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A130" s="28" t="s">
+      <c r="A130" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="B130" s="29">
+      <c r="B130" s="26">
         <v>1.1113999999999999</v>
       </c>
-      <c r="C130" s="29">
+      <c r="C130" s="26">
         <v>4.9843099999999998</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A131" s="27" t="s">
+      <c r="A131" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="B131" s="26">
+      <c r="B131" s="23">
         <v>1.6415900000000001</v>
       </c>
-      <c r="C131" s="26">
+      <c r="C131" s="23">
         <v>1.5857699999999999</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A132" s="28" t="s">
+      <c r="A132" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="B132" s="29">
+      <c r="B132" s="26">
         <v>2.17686</v>
       </c>
-      <c r="C132" s="29">
+      <c r="C132" s="26">
         <v>2.2328000000000001</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A133" s="28" t="s">
+      <c r="A133" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="B133" s="26">
+      <c r="B133" s="23">
         <v>1.17503</v>
       </c>
-      <c r="C133" s="26">
+      <c r="C133" s="23">
         <v>3.63009</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A134" s="28" t="s">
+      <c r="A134" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="B134" s="29">
+      <c r="B134" s="26">
         <v>0.87659299999999996</v>
       </c>
-      <c r="C134" s="29">
+      <c r="C134" s="26">
         <v>5.26607</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A135" s="28" t="s">
+      <c r="A135" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="B135" s="29">
+      <c r="B135" s="26">
         <v>0.84050199999999997</v>
       </c>
-      <c r="C135" s="29">
+      <c r="C135" s="26">
         <v>6.8396499999999998</v>
       </c>
     </row>

</xml_diff>